<commit_message>
Adjusting the basic structure od HSI and CYRS
As mentioned in the review sheet
CYRS and HSIs' main structure have been changed.
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -46,9 +46,6 @@
     <t>Document status section shall be a table with the following coloms  --&gt;  "Version, Date , Auther,Status "</t>
   </si>
   <si>
-    <t>24/1/2021</t>
-  </si>
-  <si>
     <t>LED String-CYRS</t>
   </si>
   <si>
@@ -101,12 +98,15 @@
   <si>
     <t>LED String-HIS</t>
   </si>
+  <si>
+    <t>Closed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,127 +164,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <condense val="0"/>
@@ -359,6 +239,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -405,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,9 +325,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,6 +360,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -646,14 +536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -661,7 +551,7 @@
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -678,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -689,13 +579,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -703,258 +593,258 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="165">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E5">
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E11">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Close the done points and adding a comment colom Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Review point</t>
   </si>
@@ -66,47 +66,57 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Requirements are taken copy paste from CYRS please provie the requirements with more details.
+    <t>Req _ LED STRING ANIMATION_PO5_CYRS _ 002 _ v01:
+Tail LEDs will be ON if Tail switch is ON and will be OFF if Tail switch is OFF
+But in CYRS the described is that Tail LEDs will be ON whatever Tail switch is ON/OFF</t>
+  </si>
+  <si>
+    <t>Req _ LED STRING ANIMATION_PO5_CYRS _ 003 _ v01 :
+Same note as previous point</t>
+  </si>
+  <si>
+    <t>24/1/2023</t>
+  </si>
+  <si>
+    <t>24/1/2024</t>
+  </si>
+  <si>
+    <t>24/1/2025</t>
+  </si>
+  <si>
+    <t>Requirements IDs shall have a diferent font different color and also version of the requirement shall be "-V01" not "_v01"</t>
+  </si>
+  <si>
+    <t>24/1/2026</t>
+  </si>
+  <si>
+    <t>LED String-HIS</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements are taken copy paste from CRS please provide the requirements with more details.
 Ex:
 Req_LED STRING ANIMATION_PO5_CYRS _ 001: describes the startup animation modes but at startup what will decide the running mode ? You should write a description of the signal/switch that decides the mode to be run, if you will implement this requirement you will run which mode? you will find your self asking about "what does make animation mode is mode 1 not 2?"   
 </t>
   </si>
   <si>
-    <t>Req _ LED STRING ANIMATION_PO5_CYRS _ 002 _ v01:
-Tail LEDs will be ON if Tail switch is ON and will be OFF if Tail switch is OFF
-But in CYRS the described is that Tail LEDs will be ON whatever Tail switch is ON/OFF</t>
-  </si>
-  <si>
-    <t>Req _ LED STRING ANIMATION_PO5_CYRS _ 003 _ v01 :
-Same note as previous point</t>
-  </si>
-  <si>
-    <t>24/1/2023</t>
-  </si>
-  <si>
-    <t>24/1/2024</t>
-  </si>
-  <si>
-    <t>24/1/2025</t>
-  </si>
-  <si>
-    <t>Requirements IDs shall have a diferent font different color and also version of the requirement shall be "-V01" not "_v01"</t>
-  </si>
-  <si>
-    <t>24/1/2026</t>
-  </si>
-  <si>
-    <t>LED String-HIS</t>
-  </si>
-  <si>
-    <t>Closed</t>
+    <t>Mali 25/1/2020: 
+Please remove "1.Project Name" no need for it</t>
+  </si>
+  <si>
+    <t>Mali 25/1/2020: Point is reviewed and closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +169,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -293,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,10 +338,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,7 +372,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -536,22 +547,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -567,8 +579,11 @@
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -585,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -599,10 +614,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -616,10 +634,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -636,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -650,10 +671,13 @@
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="165">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -664,15 +688,15 @@
         <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="75">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -681,15 +705,15 @@
         <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -698,15 +722,15 @@
         <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -715,101 +739,104 @@
         <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>

</xml_diff>

<commit_message>
Answering SIQ sheet and edit review sheet by adding new colom (Acceptance) also review the closed points Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Review" sheetId="4" r:id="rId1"/>
+    <sheet name="HSI review" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t>Review point</t>
   </si>
@@ -34,16 +35,7 @@
     <t>Point status</t>
   </si>
   <si>
-    <t>Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIQ sheet </t>
-  </si>
-  <si>
     <t>Document status section shall be a table with the following coloms  --&gt;  "Version, Date , Auther,Status "</t>
-  </si>
-  <si>
-    <t>LED String-CYRS</t>
   </si>
   <si>
     <t>24/1/2022</t>
@@ -85,9 +77,6 @@
   </si>
   <si>
     <t>24/1/2026</t>
-  </si>
-  <si>
-    <t>LED String-HIS</t>
   </si>
   <si>
     <t>Closed</t>
@@ -108,12 +97,43 @@
   <si>
     <t>Mali 25/1/2020: Point is reviewed and closed</t>
   </si>
+  <si>
+    <t>Acceptance</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: SIQ sheet ptovided with questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mali 30/1/2020: Please provide a block "Microcontroller" has input side(Input switches) and output side (LEDs) </t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>30/1/2020</t>
+  </si>
+  <si>
+    <t>Please provide all titles, tables and data with the same format of HSI 
+also the requirement ID with a diff. suitable color</t>
+  </si>
+  <si>
+    <t>Please remove curly brackets</t>
+  </si>
+  <si>
+    <t>Edit the affected requirements by SIQ sheet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,11 +190,582 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="75">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -303,7 +894,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,10 +926,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,7 +960,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -546,23 +1135,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59" customWidth="1"/>
+    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" customWidth="1"/>
+    <col min="6" max="6" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -570,316 +1159,481 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="165">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="75">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" ht="45">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E5">
-    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E2:E5 F2">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="32" priority="16" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="31" priority="17" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E11">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E7:E12">
+    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+  <conditionalFormatting sqref="D2:D12">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E14">
       <formula1>"Open, Closed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D14">
+      <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>"Accepted, Rejected"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>"Open, Closed"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update review sheet of CYRS & SRS Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
   <si>
     <t>Review point</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Edit the affected requirements by SIQ sheet</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Point is reviewed and closed</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="36">
     <dxf>
       <font>
         <condense val="0"/>
@@ -313,6 +316,13 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -323,16 +333,7 @@
     </dxf>
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -349,7 +350,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -436,334 +439,6 @@
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -1138,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1389,9 +1064,14 @@
       <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1458,77 +1138,96 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E5 F2">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="33" priority="41" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="32" priority="16" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="32" priority="21" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="17" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="31" priority="22" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E12">
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D12">
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -1608,21 +1307,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update review sheet according to CYRS updates and SRS Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Review" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Review point</t>
   </si>
@@ -91,10 +91,6 @@
 </t>
   </si>
   <si>
-    <t>Mali 25/1/2020: 
-Please remove "1.Project Name" no need for it</t>
-  </si>
-  <si>
     <t>Mali 25/1/2020: Point is reviewed and closed</t>
   </si>
   <si>
@@ -108,9 +104,6 @@
   </si>
   <si>
     <t>Mali 30/1/2020: SIQ sheet ptovided with questions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mali 30/1/2020: Please provide a block "Microcontroller" has input side(Input switches) and output side (LEDs) </t>
   </si>
   <si>
     <t>Mali 30/1/2020: Point is reviewed and closed</t>
@@ -130,6 +123,25 @@
   </si>
   <si>
     <t>Mali 6/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>Mali 30/1/2020: Please provide a block "Microcontroller" has input side(Input switches) and output side (LEDs) 
+Mali 6/2/2020: TI switch still a 3 phase switch while TI has 2 separate switches</t>
+  </si>
+  <si>
+    <t>Requirement "Req _ SEQUENCE OF TI FUNCTION RIGHT_PO5_CYRS_005-V01" &amp; "Req _ SEQUENCE OF TI FUNCTION RIGHT_PO5_CYRS_006-V01", they don't declare that scenario of TI animation is repeated till TI switch is released.</t>
+  </si>
+  <si>
+    <t>Req _ SELECT WELCOME MODE_PO5_CYRS_001-V01 doesn't declare
+the switch is Mode switch it's just saying "If the switch"</t>
+  </si>
+  <si>
+    <t>Mali 25/1/2020: 
+Please remove "1.Project Name" no need for it
+Mali6/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Pointstill open</t>
   </si>
 </sst>
 </file>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,30 +214,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
+  <dxfs count="74">
     <dxf>
       <font>
         <condense val="0"/>
@@ -316,6 +312,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -340,25 +355,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -402,6 +398,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -426,25 +441,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -469,6 +465,44 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -487,6 +521,312 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -813,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -837,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -857,16 +1197,16 @@
         <v>9</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -877,13 +1217,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -897,16 +1237,16 @@
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -918,10 +1258,10 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75">
@@ -935,13 +1275,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="165">
@@ -954,9 +1294,14 @@
       <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75">
@@ -970,13 +1315,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
@@ -990,13 +1335,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30">
@@ -1010,13 +1355,13 @@
         <v>17</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
@@ -1030,74 +1375,102 @@
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60">
+      <c r="A15" s="10">
+        <v>43984</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="45">
+      <c r="A16" s="10">
+        <v>43984</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1"/>
@@ -1138,108 +1511,165 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E5 F2">
-    <cfRule type="containsText" dxfId="35" priority="39" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="40" priority="54" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="40" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="39" priority="55" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="41" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="38" priority="56" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="32" priority="21" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="68" priority="36" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="22" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="67" priority="37" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="66" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E12">
-    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="65" priority="33" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="64" priority="34" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="63" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D12">
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="31" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="32" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E13:E14">
+    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="61" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="60" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+  <conditionalFormatting sqref="D13:D14">
+    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="27" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="57" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="56" priority="24" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="55" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E13:E14">
+    <cfRule type="containsText" dxfId="52" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="51" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="50" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="D13:D14">
+    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E16">
+    <cfRule type="containsText" dxfId="37" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="14" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E16">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E16">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1252,7 +1682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1276,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -1296,32 +1726,32 @@
         <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix CYRS points as they still not fixed (12,16) Release CYRS & HSI Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Review" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
   <si>
     <t>Review point</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Acceptance</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Accepted</t>
   </si>
   <si>
@@ -123,10 +120,6 @@
   </si>
   <si>
     <t>Mali 6/2/2020: Point is reviewed and closed</t>
-  </si>
-  <si>
-    <t>Mali 30/1/2020: Please provide a block "Microcontroller" has input side(Input switches) and output side (LEDs) 
-Mali 6/2/2020: TI switch still a 3 phase switch while TI has 2 separate switches</t>
   </si>
   <si>
     <t>Requirement "Req _ SEQUENCE OF TI FUNCTION RIGHT_PO5_CYRS_005-V01" &amp; "Req _ SEQUENCE OF TI FUNCTION RIGHT_PO5_CYRS_006-V01", they don't declare that scenario of TI animation is repeated till TI switch is released.</t>
@@ -141,7 +134,16 @@
 Mali6/2/2020: Point is reviewed and closed</t>
   </si>
   <si>
-    <t>Mali 6/2/2020: Pointstill open</t>
+    <t>Mali 30/1/2020: Please provide a block "Microcontroller" has input side(Input switches) and output side (LEDs) 
+Mali 6/2/2020: TI switch still a 3 phase switch while TI has 2 separate switches
+Mali 9/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 9/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Pointstill open
+Mali 9/2/2020: Point is closed</t>
   </si>
 </sst>
 </file>
@@ -221,7 +223,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="93">
     <dxf>
       <font>
         <condense val="0"/>
@@ -331,6 +333,215 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -355,6 +566,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -398,25 +628,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -441,6 +652,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -484,25 +714,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -527,6 +738,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -551,6 +781,25 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -637,25 +886,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
     </dxf>
@@ -784,49 +1014,6 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -1153,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1197,13 +1384,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45">
@@ -1217,13 +1404,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30">
@@ -1237,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>19</v>
@@ -1246,7 +1433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75">
+    <row r="5" spans="1:6" ht="90">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1256,12 +1443,14 @@
       <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75">
@@ -1275,7 +1464,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
@@ -1295,13 +1484,13 @@
         <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75">
@@ -1315,13 +1504,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30">
@@ -1335,13 +1524,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30">
@@ -1355,13 +1544,13 @@
         <v>17</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30">
@@ -1375,7 +1564,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>19</v>
@@ -1386,60 +1575,62 @@
     </row>
     <row r="12" spans="1:6" ht="45">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60">
@@ -1450,13 +1641,17 @@
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="45">
       <c r="A16" s="10">
@@ -1466,10 +1661,16 @@
         <v>4</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1511,115 +1712,161 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E5 F2">
-    <cfRule type="containsText" dxfId="40" priority="54" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="92" priority="66" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="55" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="91" priority="67" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="56" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="90" priority="68" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="68" priority="36" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="89" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="37" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="88" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="38" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="87" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E12">
-    <cfRule type="containsText" dxfId="65" priority="33" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="86" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="34" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="85" priority="46" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="84" priority="47" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D12">
-    <cfRule type="cellIs" dxfId="42" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="43" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="44" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:E14">
-    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E13:E16">
+    <cfRule type="containsText" dxfId="81" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="80" priority="41" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="79" priority="42" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D14">
-    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
+  <conditionalFormatting sqref="D13:D15">
+    <cfRule type="cellIs" dxfId="78" priority="38" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="57" priority="23" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E14:E16">
+    <cfRule type="containsText" dxfId="76" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="24" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="75" priority="36" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="25" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="74" priority="37" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
+  <conditionalFormatting sqref="D14:D15">
+    <cfRule type="cellIs" dxfId="73" priority="33" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="34" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:E14">
-    <cfRule type="containsText" dxfId="52" priority="18" operator="containsText" text="Open">
+  <conditionalFormatting sqref="E13:E16">
+    <cfRule type="containsText" dxfId="71" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="19" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="70" priority="31" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="69" priority="32" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D14">
-    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
+  <conditionalFormatting sqref="D13:D15">
+    <cfRule type="cellIs" dxfId="68" priority="28" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="29" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E16">
-    <cfRule type="containsText" dxfId="37" priority="13" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="66" priority="25" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="14" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="65" priority="26" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="64" priority="27" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="63" priority="23" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="24" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E16">
+    <cfRule type="containsText" dxfId="61" priority="20" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="21" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="22" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="58" priority="18" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="19" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E16">
+    <cfRule type="containsText" dxfId="56" priority="15" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="16" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="17" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="53" priority="13" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="14" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -1627,37 +1874,39 @@
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E16">
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E16">
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -1669,7 +1918,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1682,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1726,7 +1975,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
@@ -1737,21 +1986,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="50" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="49" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="70" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>